<commit_message>
revision of sbl presentation.
</commit_message>
<xml_diff>
--- a/proiel/rResults/rel_Gospels_Nov16.xlsx
+++ b/proiel/rResults/rel_Gospels_Nov16.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="360" windowWidth="17940" windowHeight="6560" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="420" windowWidth="17940" windowHeight="6495" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2477" uniqueCount="622">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2544" uniqueCount="629">
   <si>
     <t>1Corinthians</t>
   </si>
@@ -1883,12 +1884,46 @@
   <si>
     <t>#-pred*obl*atr / #-pred</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">#-pred*xadv / </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>-pred</t>
+    </r>
+  </si>
+  <si>
+    <t>#-pred*xobj / #-pred</t>
+  </si>
+  <si>
+    <t>#-pred*sub*sub / #-pred</t>
+  </si>
+  <si>
+    <t>#-pred*sub*sub / #-pred*sub</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>#-pred*adv*obl / #-pred</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2020,6 +2055,14 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2711,625 +2754,624 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:ASY21"/>
+  <dimension ref="A1:ASY23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="P4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="T1" sqref="T1:U21"/>
+      <selection pane="bottomRight" activeCell="H1" sqref="H1:I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="20" max="21" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="26" max="31" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="33" width="15" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="38" max="39" width="15" bestFit="1" customWidth="1"/>
-    <col min="40" max="41" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="42" max="43" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="40" max="41" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="12" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="48" max="49" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="50" max="51" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="52" max="53" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="54" max="55" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="62" max="63" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="64" max="65" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="66" max="67" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="68" max="69" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="71" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="72" max="73" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="74" max="75" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="49" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="51" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="53" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="54" max="55" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="56" max="57" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="62" max="63" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="65" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="66" max="67" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="68" max="69" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="73" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="74" max="75" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="76" max="77" width="15" bestFit="1" customWidth="1"/>
-    <col min="78" max="79" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="80" max="81" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="82" max="83" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="84" max="85" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="86" max="87" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="88" max="89" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="90" max="91" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="92" max="93" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="94" max="95" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="96" max="97" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="98" max="99" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="100" max="101" width="14.36328125" bestFit="1" customWidth="1"/>
-    <col min="102" max="103" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="104" max="105" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="78" max="79" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="80" max="81" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="82" max="83" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="84" max="85" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="86" max="87" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="88" max="89" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="90" max="91" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="92" max="93" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="94" max="95" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="96" max="97" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="98" max="101" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="102" max="103" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="104" max="105" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="106" max="107" width="15" bestFit="1" customWidth="1"/>
-    <col min="108" max="109" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="108" max="109" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="110" max="111" width="20" bestFit="1" customWidth="1"/>
-    <col min="112" max="113" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="114" max="115" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="116" max="117" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="118" max="119" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="112" max="113" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="114" max="115" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="116" max="117" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="118" max="119" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="120" max="121" width="15" bestFit="1" customWidth="1"/>
-    <col min="122" max="123" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="124" max="125" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="126" max="127" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="128" max="129" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="130" max="131" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="132" max="133" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="134" max="135" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="136" max="137" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="138" max="139" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="140" max="141" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="142" max="143" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="144" max="145" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="147" max="147" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="148" max="149" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="150" max="151" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="152" max="153" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="154" max="155" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="156" max="157" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="158" max="159" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="160" max="161" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="162" max="163" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="164" max="165" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="166" max="167" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="168" max="169" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="170" max="171" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="172" max="173" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="174" max="175" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="176" max="177" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="122" max="123" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="124" max="125" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="126" max="127" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="128" max="129" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="130" max="131" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="132" max="133" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="134" max="135" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="136" max="137" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="138" max="139" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="140" max="141" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="142" max="143" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="144" max="145" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="148" max="149" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="150" max="151" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="152" max="153" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="154" max="155" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="156" max="157" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="158" max="159" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="160" max="161" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="162" max="163" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="164" max="165" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="166" max="167" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="168" max="169" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="170" max="171" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="172" max="173" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="174" max="175" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="176" max="177" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="178" max="179" width="15" bestFit="1" customWidth="1"/>
-    <col min="180" max="181" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="182" max="183" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="184" max="185" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="186" max="187" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="188" max="189" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="190" max="191" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="192" max="193" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="194" max="195" width="16.26953125" bestFit="1" customWidth="1"/>
-    <col min="196" max="197" width="22.08984375" bestFit="1" customWidth="1"/>
+    <col min="180" max="181" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="182" max="183" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="184" max="185" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="186" max="187" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="188" max="189" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="190" max="191" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="192" max="193" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="194" max="195" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="196" max="197" width="22.140625" bestFit="1" customWidth="1"/>
     <col min="198" max="199" width="20" bestFit="1" customWidth="1"/>
-    <col min="200" max="201" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="202" max="203" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="204" max="204" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="205" max="205" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="206" max="207" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="208" max="209" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="210" max="211" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="212" max="213" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="214" max="215" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="200" max="201" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="202" max="203" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="204" max="204" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="205" max="205" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="206" max="207" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="208" max="209" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="210" max="211" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="212" max="213" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="214" max="215" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="216" max="217" width="19" bestFit="1" customWidth="1"/>
-    <col min="218" max="219" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="220" max="221" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="222" max="223" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="224" max="225" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="226" max="227" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="228" max="229" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="230" max="231" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="232" max="233" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="234" max="235" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="236" max="237" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="238" max="239" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="240" max="241" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="242" max="243" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="244" max="245" width="30.6328125" bestFit="1" customWidth="1"/>
-    <col min="246" max="247" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="248" max="249" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="250" max="251" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="254" max="255" width="15.08984375" bestFit="1" customWidth="1"/>
-    <col min="256" max="257" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="258" max="259" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="260" max="261" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="262" max="263" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="264" max="265" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="266" max="267" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="268" max="269" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="270" max="271" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="272" max="273" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="274" max="275" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="218" max="219" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="220" max="221" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="222" max="223" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="224" max="225" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="226" max="227" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="228" max="229" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="230" max="231" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="232" max="233" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="234" max="235" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="236" max="237" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="238" max="239" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="240" max="241" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="242" max="243" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="244" max="245" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="246" max="247" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="248" max="249" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="250" max="251" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="253" max="253" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="254" max="255" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="256" max="257" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="258" max="259" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="260" max="261" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="262" max="263" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="264" max="265" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="266" max="267" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="268" max="269" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="270" max="271" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="272" max="273" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="274" max="275" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="276" max="277" width="23" bestFit="1" customWidth="1"/>
-    <col min="278" max="279" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="280" max="281" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="282" max="283" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="284" max="285" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="286" max="287" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="288" max="289" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="290" max="291" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="292" max="293" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="294" max="295" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="296" max="297" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="298" max="299" width="21.7265625" bestFit="1" customWidth="1"/>
-    <col min="300" max="301" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="302" max="303" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="304" max="305" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="278" max="279" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="280" max="281" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="282" max="283" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="284" max="285" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="286" max="287" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="288" max="289" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="290" max="291" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="292" max="293" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="294" max="295" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="296" max="297" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="298" max="299" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="300" max="301" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="302" max="303" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="304" max="305" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="306" max="307" width="20" bestFit="1" customWidth="1"/>
-    <col min="308" max="309" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="310" max="311" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="312" max="313" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="314" max="315" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="308" max="309" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="310" max="311" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="312" max="313" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="314" max="315" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="316" max="317" width="20" bestFit="1" customWidth="1"/>
-    <col min="318" max="319" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="320" max="321" width="15.36328125" bestFit="1" customWidth="1"/>
-    <col min="322" max="323" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="324" max="325" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="326" max="327" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="328" max="329" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="330" max="333" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="334" max="335" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="336" max="337" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="338" max="339" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="340" max="341" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="342" max="343" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="344" max="345" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="346" max="347" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="348" max="349" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="350" max="351" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="352" max="353" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="354" max="355" width="19.6328125" bestFit="1" customWidth="1"/>
-    <col min="356" max="357" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="358" max="359" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="318" max="319" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="320" max="321" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="322" max="323" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="324" max="325" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="326" max="327" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="328" max="329" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="330" max="333" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="334" max="335" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="336" max="337" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="338" max="339" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="340" max="341" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="342" max="343" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="344" max="345" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="346" max="347" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="348" max="349" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="350" max="351" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="352" max="353" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="354" max="355" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="356" max="357" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="358" max="359" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="360" max="361" width="20" bestFit="1" customWidth="1"/>
-    <col min="362" max="363" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="364" max="365" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="366" max="367" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="368" max="369" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="370" max="371" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="372" max="373" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="374" max="375" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="362" max="363" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="364" max="365" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="366" max="367" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="368" max="369" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="370" max="371" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="372" max="373" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="374" max="375" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="376" max="377" width="23" bestFit="1" customWidth="1"/>
-    <col min="378" max="379" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="380" max="381" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="382" max="383" width="22.81640625" bestFit="1" customWidth="1"/>
+    <col min="378" max="379" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="380" max="381" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="382" max="383" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="384" max="385" width="16" bestFit="1" customWidth="1"/>
-    <col min="386" max="387" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="388" max="389" width="36.1796875" bestFit="1" customWidth="1"/>
-    <col min="390" max="391" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="392" max="393" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="394" max="395" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="396" max="397" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="398" max="399" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="400" max="401" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="402" max="403" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="404" max="405" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="406" max="407" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="408" max="409" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="410" max="411" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="412" max="413" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="414" max="415" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="416" max="417" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="418" max="419" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="420" max="421" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="386" max="387" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="388" max="389" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="390" max="391" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="392" max="393" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="394" max="395" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="396" max="397" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="398" max="399" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="400" max="401" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="402" max="403" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="404" max="405" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="406" max="407" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="408" max="409" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="410" max="411" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="412" max="413" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="414" max="415" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="416" max="417" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="418" max="419" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="420" max="421" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="422" max="423" width="27" bestFit="1" customWidth="1"/>
-    <col min="424" max="425" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="426" max="427" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="428" max="429" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="430" max="431" width="20.36328125" bestFit="1" customWidth="1"/>
+    <col min="424" max="425" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="426" max="427" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="428" max="429" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="430" max="431" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="432" max="433" width="22" bestFit="1" customWidth="1"/>
-    <col min="434" max="435" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="436" max="437" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="438" max="439" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="440" max="441" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="442" max="443" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="444" max="445" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="446" max="447" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="448" max="449" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="450" max="451" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="452" max="453" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="454" max="455" width="57.7265625" bestFit="1" customWidth="1"/>
-    <col min="456" max="457" width="31.453125" bestFit="1" customWidth="1"/>
-    <col min="458" max="459" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="460" max="461" width="18.7265625" bestFit="1" customWidth="1"/>
-    <col min="462" max="465" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="466" max="467" width="59.90625" bestFit="1" customWidth="1"/>
-    <col min="468" max="469" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="470" max="471" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="472" max="473" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="474" max="475" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="476" max="477" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="478" max="479" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="480" max="481" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="482" max="483" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="484" max="485" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="486" max="487" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="488" max="489" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="490" max="491" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="492" max="493" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="494" max="495" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="434" max="435" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="436" max="437" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="438" max="439" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="440" max="441" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="442" max="443" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="444" max="445" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="446" max="447" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="448" max="449" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="450" max="451" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="452" max="453" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="454" max="455" width="57.7109375" bestFit="1" customWidth="1"/>
+    <col min="456" max="457" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="458" max="459" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="460" max="461" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="462" max="465" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="466" max="467" width="59.85546875" bestFit="1" customWidth="1"/>
+    <col min="468" max="469" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="470" max="471" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="472" max="473" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="474" max="475" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="476" max="477" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="478" max="479" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="480" max="481" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="482" max="483" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="484" max="485" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="486" max="487" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="488" max="489" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="490" max="491" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="492" max="493" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="494" max="495" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="496" max="497" width="20" bestFit="1" customWidth="1"/>
-    <col min="498" max="499" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="500" max="501" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="502" max="503" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="504" max="505" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="506" max="507" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="508" max="509" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="510" max="511" width="27.6328125" bestFit="1" customWidth="1"/>
-    <col min="512" max="513" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="514" max="515" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="498" max="499" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="500" max="501" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="502" max="503" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="504" max="505" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="506" max="507" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="508" max="509" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="510" max="511" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="512" max="513" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="514" max="515" width="25.85546875" bestFit="1" customWidth="1"/>
     <col min="516" max="517" width="28" bestFit="1" customWidth="1"/>
-    <col min="518" max="521" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="522" max="523" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="518" max="521" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="522" max="523" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="524" max="525" width="20" bestFit="1" customWidth="1"/>
-    <col min="526" max="527" width="26.36328125" bestFit="1" customWidth="1"/>
-    <col min="528" max="529" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="530" max="531" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="532" max="533" width="19.6328125" bestFit="1" customWidth="1"/>
+    <col min="526" max="527" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="528" max="529" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="530" max="531" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="532" max="533" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="534" max="535" width="25" bestFit="1" customWidth="1"/>
-    <col min="536" max="537" width="28.26953125" bestFit="1" customWidth="1"/>
-    <col min="538" max="539" width="34.7265625" bestFit="1" customWidth="1"/>
-    <col min="540" max="541" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="536" max="537" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="538" max="539" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="540" max="541" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="542" max="543" width="24" bestFit="1" customWidth="1"/>
-    <col min="544" max="545" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="546" max="547" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="548" max="549" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="550" max="551" width="28.90625" bestFit="1" customWidth="1"/>
-    <col min="552" max="553" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="554" max="555" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="556" max="557" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="558" max="559" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="560" max="561" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="562" max="563" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="564" max="565" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="566" max="567" width="18.453125" bestFit="1" customWidth="1"/>
-    <col min="568" max="569" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="570" max="571" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="572" max="573" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="574" max="575" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="576" max="577" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="578" max="579" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="580" max="581" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="582" max="583" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="584" max="585" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="586" max="587" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="544" max="545" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="546" max="547" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="548" max="549" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="550" max="551" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="552" max="553" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="554" max="555" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="556" max="557" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="558" max="559" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="560" max="561" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="562" max="563" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="564" max="565" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="566" max="567" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="568" max="569" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="570" max="571" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="572" max="573" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="574" max="575" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="576" max="577" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="578" max="579" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="580" max="581" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="582" max="583" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="584" max="585" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="586" max="587" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="588" max="589" width="20" bestFit="1" customWidth="1"/>
-    <col min="590" max="591" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="592" max="593" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="594" max="594" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="595" max="595" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="596" max="597" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="598" max="599" width="29.26953125" bestFit="1" customWidth="1"/>
-    <col min="600" max="601" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="602" max="603" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="604" max="605" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="606" max="607" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="608" max="609" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="610" max="611" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="612" max="613" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="614" max="615" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="616" max="617" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="618" max="619" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="620" max="621" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="622" max="623" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="624" max="625" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="590" max="591" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="592" max="593" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="594" max="594" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="595" max="595" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="596" max="597" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="598" max="599" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="600" max="601" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="602" max="603" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="604" max="605" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="606" max="607" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="608" max="609" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="610" max="611" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="612" max="613" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="614" max="615" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="616" max="617" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="618" max="619" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="620" max="621" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="622" max="623" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="624" max="625" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="626" max="627" width="20" bestFit="1" customWidth="1"/>
-    <col min="628" max="629" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="630" max="631" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="632" max="633" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="634" max="635" width="20.6328125" bestFit="1" customWidth="1"/>
-    <col min="636" max="637" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="638" max="639" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="640" max="641" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="642" max="643" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="644" max="645" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="646" max="647" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="648" max="649" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="650" max="651" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="652" max="653" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="654" max="655" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="656" max="657" width="30.36328125" bestFit="1" customWidth="1"/>
-    <col min="658" max="659" width="34.08984375" bestFit="1" customWidth="1"/>
-    <col min="660" max="661" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="662" max="663" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="664" max="665" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="666" max="667" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="668" max="669" width="35.36328125" bestFit="1" customWidth="1"/>
-    <col min="670" max="671" width="50.26953125" bestFit="1" customWidth="1"/>
-    <col min="672" max="673" width="53.6328125" bestFit="1" customWidth="1"/>
-    <col min="674" max="675" width="61.453125" bestFit="1" customWidth="1"/>
-    <col min="676" max="677" width="54.36328125" bestFit="1" customWidth="1"/>
-    <col min="678" max="679" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="680" max="683" width="37.26953125" bestFit="1" customWidth="1"/>
-    <col min="684" max="685" width="36.90625" bestFit="1" customWidth="1"/>
-    <col min="686" max="687" width="40.6328125" bestFit="1" customWidth="1"/>
-    <col min="688" max="689" width="35.1796875" bestFit="1" customWidth="1"/>
-    <col min="690" max="691" width="38.1796875" bestFit="1" customWidth="1"/>
-    <col min="692" max="693" width="33.7265625" bestFit="1" customWidth="1"/>
-    <col min="694" max="695" width="37.08984375" bestFit="1" customWidth="1"/>
-    <col min="696" max="697" width="37.81640625" bestFit="1" customWidth="1"/>
-    <col min="698" max="699" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="700" max="701" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="702" max="703" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="628" max="629" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="630" max="631" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="632" max="633" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="634" max="635" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="636" max="637" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="638" max="639" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="640" max="641" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="642" max="643" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="644" max="645" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="646" max="647" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="648" max="649" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="650" max="651" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="652" max="653" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="654" max="655" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="656" max="657" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="658" max="659" width="34.140625" bestFit="1" customWidth="1"/>
+    <col min="660" max="661" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="662" max="663" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="664" max="665" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="666" max="667" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="668" max="669" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="670" max="671" width="50.28515625" bestFit="1" customWidth="1"/>
+    <col min="672" max="673" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="674" max="675" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="676" max="677" width="54.42578125" bestFit="1" customWidth="1"/>
+    <col min="678" max="679" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="680" max="683" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="684" max="685" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="686" max="687" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="688" max="689" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="690" max="691" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="692" max="693" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="694" max="695" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="696" max="697" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="698" max="699" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="700" max="701" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="702" max="703" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="704" max="705" width="28" bestFit="1" customWidth="1"/>
-    <col min="706" max="707" width="21.36328125" bestFit="1" customWidth="1"/>
-    <col min="708" max="709" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="706" max="707" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="708" max="709" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="710" max="711" width="20" bestFit="1" customWidth="1"/>
-    <col min="712" max="713" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="714" max="715" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="716" max="717" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="718" max="719" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="720" max="721" width="25.81640625" bestFit="1" customWidth="1"/>
-    <col min="722" max="723" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="724" max="725" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="726" max="727" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="728" max="729" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="730" max="731" width="20.54296875" bestFit="1" customWidth="1"/>
-    <col min="732" max="733" width="22.90625" bestFit="1" customWidth="1"/>
+    <col min="712" max="713" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="714" max="715" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="716" max="717" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="718" max="719" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="720" max="721" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="722" max="723" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="724" max="725" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="726" max="727" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="728" max="729" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="730" max="731" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="732" max="733" width="22.85546875" bestFit="1" customWidth="1"/>
     <col min="734" max="735" width="15" bestFit="1" customWidth="1"/>
-    <col min="736" max="737" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="736" max="737" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="738" max="739" width="20" bestFit="1" customWidth="1"/>
-    <col min="740" max="741" width="30.26953125" bestFit="1" customWidth="1"/>
-    <col min="742" max="743" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="744" max="745" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="746" max="747" width="23.90625" bestFit="1" customWidth="1"/>
-    <col min="748" max="749" width="25.453125" bestFit="1" customWidth="1"/>
-    <col min="750" max="751" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="752" max="753" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="754" max="755" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="740" max="741" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="742" max="743" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="744" max="745" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="746" max="747" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="748" max="749" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="750" max="751" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="752" max="753" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="754" max="755" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="756" max="757" width="22" bestFit="1" customWidth="1"/>
-    <col min="758" max="759" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="760" max="761" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="762" max="763" width="19.90625" bestFit="1" customWidth="1"/>
-    <col min="764" max="765" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="766" max="767" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="768" max="769" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="770" max="771" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="772" max="773" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="774" max="775" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="776" max="777" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="778" max="779" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="780" max="781" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="782" max="783" width="24.6328125" bestFit="1" customWidth="1"/>
-    <col min="784" max="785" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="786" max="787" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="788" max="789" width="17.1796875" bestFit="1" customWidth="1"/>
-    <col min="790" max="791" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="792" max="793" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="794" max="795" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="796" max="797" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="798" max="799" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="800" max="801" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="802" max="803" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="804" max="805" width="29.7265625" bestFit="1" customWidth="1"/>
+    <col min="758" max="759" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="760" max="761" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="762" max="763" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="764" max="765" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="766" max="767" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="768" max="769" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="770" max="771" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="772" max="773" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="774" max="775" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="776" max="777" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="778" max="779" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="780" max="781" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="782" max="783" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="784" max="785" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="786" max="787" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="788" max="789" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="790" max="791" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="792" max="793" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="794" max="795" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="796" max="797" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="798" max="799" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="800" max="801" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="802" max="803" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="804" max="805" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="806" max="807" width="24" bestFit="1" customWidth="1"/>
-    <col min="808" max="809" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="810" max="811" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="812" max="813" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="814" max="815" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="816" max="817" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="818" max="819" width="30.7265625" bestFit="1" customWidth="1"/>
-    <col min="820" max="821" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="822" max="823" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="824" max="825" width="21.1796875" bestFit="1" customWidth="1"/>
-    <col min="826" max="827" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="828" max="829" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="830" max="831" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="832" max="833" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="834" max="835" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="808" max="809" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="810" max="811" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="812" max="813" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="814" max="815" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="816" max="817" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="818" max="819" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="820" max="821" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="822" max="823" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="824" max="825" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="826" max="827" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="828" max="829" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="830" max="831" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="832" max="833" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="834" max="835" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="836" max="837" width="26" bestFit="1" customWidth="1"/>
-    <col min="838" max="839" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="840" max="841" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="842" max="843" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="844" max="845" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="846" max="847" width="22.54296875" bestFit="1" customWidth="1"/>
+    <col min="838" max="839" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="840" max="841" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="842" max="843" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="844" max="845" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="846" max="847" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="848" max="849" width="24" bestFit="1" customWidth="1"/>
-    <col min="850" max="851" width="26.1796875" bestFit="1" customWidth="1"/>
-    <col min="852" max="853" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="854" max="855" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="856" max="857" width="28.7265625" bestFit="1" customWidth="1"/>
-    <col min="858" max="859" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="860" max="861" width="32.08984375" bestFit="1" customWidth="1"/>
-    <col min="862" max="863" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="864" max="865" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="866" max="867" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="868" max="869" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="870" max="871" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="850" max="851" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="852" max="853" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="854" max="855" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="856" max="857" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="858" max="859" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="860" max="861" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="862" max="863" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="864" max="865" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="866" max="867" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="868" max="869" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="870" max="871" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="872" max="873" width="15" bestFit="1" customWidth="1"/>
-    <col min="874" max="875" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="876" max="877" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="878" max="879" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="880" max="881" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="874" max="875" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="876" max="877" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="878" max="879" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="880" max="881" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="882" max="883" width="25" bestFit="1" customWidth="1"/>
     <col min="884" max="885" width="28" bestFit="1" customWidth="1"/>
-    <col min="886" max="887" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="888" max="889" width="16.81640625" bestFit="1" customWidth="1"/>
-    <col min="890" max="891" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="892" max="893" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="894" max="895" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="896" max="897" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="886" max="887" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="888" max="889" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="890" max="891" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="892" max="893" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="894" max="895" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="896" max="897" width="24.42578125" bestFit="1" customWidth="1"/>
     <col min="898" max="899" width="25" bestFit="1" customWidth="1"/>
-    <col min="900" max="901" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="902" max="903" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="904" max="905" width="29.54296875" bestFit="1" customWidth="1"/>
-    <col min="906" max="907" width="45.6328125" bestFit="1" customWidth="1"/>
-    <col min="908" max="909" width="31.08984375" bestFit="1" customWidth="1"/>
-    <col min="910" max="911" width="38.81640625" bestFit="1" customWidth="1"/>
-    <col min="912" max="913" width="39.453125" bestFit="1" customWidth="1"/>
-    <col min="914" max="915" width="22.54296875" bestFit="1" customWidth="1"/>
-    <col min="916" max="917" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="918" max="919" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="920" max="921" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="922" max="923" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="900" max="901" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="902" max="903" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="904" max="905" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="906" max="907" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="908" max="909" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="910" max="911" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="912" max="913" width="39.42578125" bestFit="1" customWidth="1"/>
+    <col min="914" max="915" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="916" max="917" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="918" max="919" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="920" max="921" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="922" max="923" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="924" max="925" width="25" bestFit="1" customWidth="1"/>
-    <col min="926" max="927" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="928" max="929" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="930" max="931" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="932" max="933" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="934" max="935" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="936" max="937" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="938" max="939" width="26.26953125" bestFit="1" customWidth="1"/>
-    <col min="940" max="941" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="942" max="943" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="944" max="945" width="22.6328125" bestFit="1" customWidth="1"/>
-    <col min="946" max="947" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="948" max="949" width="25.453125" bestFit="1" customWidth="1"/>
+    <col min="926" max="927" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="928" max="929" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="930" max="931" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="932" max="933" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="934" max="935" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="936" max="937" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="938" max="939" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="940" max="941" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="942" max="943" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="944" max="945" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="946" max="947" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="948" max="949" width="25.42578125" bestFit="1" customWidth="1"/>
     <col min="950" max="951" width="20" bestFit="1" customWidth="1"/>
-    <col min="952" max="953" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="954" max="955" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="956" max="957" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="958" max="959" width="28.54296875" bestFit="1" customWidth="1"/>
-    <col min="960" max="961" width="26.08984375" bestFit="1" customWidth="1"/>
-    <col min="962" max="963" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="964" max="965" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="966" max="967" width="26.54296875" bestFit="1" customWidth="1"/>
-    <col min="968" max="969" width="24.453125" bestFit="1" customWidth="1"/>
-    <col min="970" max="971" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="952" max="953" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="954" max="955" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="956" max="957" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="958" max="959" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="960" max="961" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="962" max="963" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="964" max="965" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="966" max="967" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="968" max="969" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="970" max="971" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="972" max="973" width="26" bestFit="1" customWidth="1"/>
-    <col min="974" max="975" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="976" max="977" width="27.08984375" bestFit="1" customWidth="1"/>
-    <col min="978" max="979" width="32.453125" bestFit="1" customWidth="1"/>
-    <col min="980" max="981" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="982" max="983" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="984" max="985" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="986" max="987" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="988" max="989" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="990" max="991" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="992" max="993" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="994" max="995" width="17.81640625" bestFit="1" customWidth="1"/>
-    <col min="996" max="997" width="21.6328125" bestFit="1" customWidth="1"/>
-    <col min="998" max="999" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="1000" max="1001" width="32.90625" bestFit="1" customWidth="1"/>
-    <col min="1002" max="1003" width="16.6328125" bestFit="1" customWidth="1"/>
-    <col min="1004" max="1005" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="1006" max="1007" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="1008" max="1009" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="1010" max="1011" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="1012" max="1013" width="43.7265625" bestFit="1" customWidth="1"/>
-    <col min="1014" max="1015" width="47.453125" bestFit="1" customWidth="1"/>
-    <col min="1016" max="1017" width="31.90625" bestFit="1" customWidth="1"/>
-    <col min="1018" max="1019" width="20.90625" bestFit="1" customWidth="1"/>
-    <col min="1020" max="1021" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="1022" max="1023" width="29.08984375" bestFit="1" customWidth="1"/>
-    <col min="1024" max="1025" width="28.453125" bestFit="1" customWidth="1"/>
-    <col min="1026" max="1027" width="21.54296875" bestFit="1" customWidth="1"/>
-    <col min="1028" max="1029" width="18.81640625" bestFit="1" customWidth="1"/>
-    <col min="1030" max="1031" width="24.81640625" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1033" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="1034" max="1035" width="23.36328125" bestFit="1" customWidth="1"/>
-    <col min="1036" max="1037" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="1038" max="1041" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="1042" max="1042" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="1043" max="1043" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="974" max="975" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="976" max="977" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="978" max="979" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="980" max="981" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="982" max="983" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="984" max="985" width="25.42578125" bestFit="1" customWidth="1"/>
+    <col min="986" max="987" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="988" max="989" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="990" max="991" width="21.28515625" bestFit="1" customWidth="1"/>
+    <col min="992" max="993" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="994" max="995" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="996" max="997" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="998" max="999" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1000" max="1001" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="1002" max="1003" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="1004" max="1005" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1006" max="1007" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1008" max="1009" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="1010" max="1011" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1012" max="1013" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="1014" max="1015" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="1016" max="1017" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1018" max="1019" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1020" max="1021" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1022" max="1023" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="1024" max="1025" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1026" max="1027" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="1028" max="1029" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="1030" max="1031" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1032" max="1033" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1034" max="1035" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1036" max="1037" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="1038" max="1041" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1042" max="1042" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1043" max="1043" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="1044" max="1045" width="27" bestFit="1" customWidth="1"/>
-    <col min="1046" max="1047" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="1048" max="1049" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="1050" max="1051" width="49.7265625" bestFit="1" customWidth="1"/>
-    <col min="1052" max="1053" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="1054" max="1055" width="26.90625" bestFit="1" customWidth="1"/>
-    <col min="1056" max="1057" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="1058" max="1059" width="27.7265625" bestFit="1" customWidth="1"/>
-    <col min="1060" max="1061" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="1062" max="1063" width="22.453125" bestFit="1" customWidth="1"/>
+    <col min="1046" max="1047" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1048" max="1049" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1050" max="1051" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="1052" max="1053" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1054" max="1055" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1056" max="1057" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="1058" max="1059" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1060" max="1061" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="1062" max="1063" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="1064" max="1065" width="25" bestFit="1" customWidth="1"/>
-    <col min="1066" max="1067" width="25.90625" bestFit="1" customWidth="1"/>
-    <col min="1068" max="1069" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="1066" max="1067" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="1068" max="1069" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="1070" max="1071" width="20" bestFit="1" customWidth="1"/>
-    <col min="1072" max="1073" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="1074" max="1075" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="1076" max="1077" width="26.7265625" bestFit="1" customWidth="1"/>
-    <col min="1078" max="1079" width="19.81640625" bestFit="1" customWidth="1"/>
-    <col min="1080" max="1081" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="1082" max="1083" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="1084" max="1085" width="32.90625" bestFit="1" customWidth="1"/>
-    <col min="1086" max="1087" width="17.08984375" bestFit="1" customWidth="1"/>
-    <col min="1088" max="1089" width="27.90625" bestFit="1" customWidth="1"/>
+    <col min="1072" max="1073" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1074" max="1075" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1076" max="1077" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1078" max="1079" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="1080" max="1081" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1082" max="1083" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1084" max="1085" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="1086" max="1087" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="1088" max="1089" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="1090" max="1091" width="25" bestFit="1" customWidth="1"/>
-    <col min="1092" max="1093" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="1094" max="1095" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="1096" max="1097" width="23.81640625" bestFit="1" customWidth="1"/>
-    <col min="1098" max="1099" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="1100" max="1101" width="24.54296875" bestFit="1" customWidth="1"/>
-    <col min="1102" max="1103" width="26.6328125" bestFit="1" customWidth="1"/>
-    <col min="1104" max="1105" width="29.90625" bestFit="1" customWidth="1"/>
-    <col min="1106" max="1107" width="23.08984375" bestFit="1" customWidth="1"/>
-    <col min="1108" max="1109" width="24.26953125" bestFit="1" customWidth="1"/>
-    <col min="1110" max="1111" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="1092" max="1093" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1094" max="1095" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1096" max="1097" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="1098" max="1099" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="1100" max="1101" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="1102" max="1103" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="1104" max="1105" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="1106" max="1107" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="1108" max="1109" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1110" max="1111" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="1112" max="1113" width="15" bestFit="1" customWidth="1"/>
-    <col min="1114" max="1115" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="1116" max="1117" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="1118" max="1119" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="1120" max="1121" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="1122" max="1123" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="1124" max="1125" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="1126" max="1126" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="1127" max="1127" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="1128" max="1129" width="22.81640625" bestFit="1" customWidth="1"/>
-    <col min="1130" max="1131" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="1132" max="1133" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="1134" max="1135" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="1136" max="1137" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="1138" max="1139" width="27.54296875" bestFit="1" customWidth="1"/>
-    <col min="1140" max="1141" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="1142" max="1143" width="23.7265625" bestFit="1" customWidth="1"/>
-    <col min="1144" max="1145" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="1146" max="1147" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="1148" max="1149" width="20.36328125" bestFit="1" customWidth="1"/>
-    <col min="1150" max="1151" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="1152" max="1153" width="28.36328125" bestFit="1" customWidth="1"/>
-    <col min="1154" max="1155" width="22.453125" bestFit="1" customWidth="1"/>
-    <col min="1156" max="1157" width="20.08984375" bestFit="1" customWidth="1"/>
-    <col min="1158" max="1159" width="20.81640625" bestFit="1" customWidth="1"/>
-    <col min="1160" max="1161" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="1162" max="1163" width="20.26953125" bestFit="1" customWidth="1"/>
-    <col min="1164" max="1165" width="22.08984375" bestFit="1" customWidth="1"/>
-    <col min="1166" max="1167" width="31.90625" bestFit="1" customWidth="1"/>
-    <col min="1168" max="1169" width="29.453125" bestFit="1" customWidth="1"/>
-    <col min="1170" max="1171" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="1114" max="1115" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1116" max="1117" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1118" max="1119" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1120" max="1121" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1122" max="1123" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="1124" max="1125" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1126" max="1126" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="1127" max="1127" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1128" max="1129" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1130" max="1131" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1132" max="1133" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1134" max="1135" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1136" max="1137" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="1138" max="1139" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1140" max="1141" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="1142" max="1143" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1144" max="1145" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="1146" max="1147" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1148" max="1149" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="1150" max="1151" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1152" max="1153" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="1154" max="1155" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="1156" max="1157" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1158" max="1159" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="1160" max="1161" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1162" max="1163" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="1164" max="1165" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="1166" max="1167" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1168" max="1169" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="1170" max="1171" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="1172" max="1173" width="26" bestFit="1" customWidth="1"/>
-    <col min="1174" max="1175" width="22.90625" bestFit="1" customWidth="1"/>
-    <col min="1176" max="1177" width="25.6328125" bestFit="1" customWidth="1"/>
-    <col min="1178" max="1179" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="1180" max="1181" width="24.08984375" bestFit="1" customWidth="1"/>
-    <col min="1182" max="1183" width="21.90625" bestFit="1" customWidth="1"/>
-    <col min="1184" max="1185" width="23.453125" bestFit="1" customWidth="1"/>
-    <col min="1186" max="1187" width="31.36328125" bestFit="1" customWidth="1"/>
-    <col min="1188" max="1189" width="18.1796875" bestFit="1" customWidth="1"/>
-    <col min="1190" max="1191" width="23.26953125" bestFit="1" customWidth="1"/>
-    <col min="1192" max="1193" width="52.54296875" bestFit="1" customWidth="1"/>
-    <col min="1194" max="1195" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="1174" max="1175" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="1176" max="1177" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="1178" max="1179" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1180" max="1181" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="1182" max="1183" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1184" max="1185" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="1186" max="1187" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="1188" max="1189" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="1190" max="1191" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1192" max="1193" width="52.5703125" bestFit="1" customWidth="1"/>
+    <col min="1194" max="1195" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1195" x14ac:dyDescent="0.35">
@@ -78648,6 +78690,12 @@
       </c>
       <c r="ASY21">
         <v>-0.28461907237941703</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1195" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <f>SMALL(B21:GS21,5)</f>
+        <v>-0.85833805195031099</v>
       </c>
     </row>
   </sheetData>
@@ -78657,21 +78705,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W24"/>
+  <dimension ref="A1:AT24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="AB4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" sqref="A1:C24"/>
+      <selection pane="bottomRight" activeCell="AQ1" sqref="AQ1:AR21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B1">
         <v>1</v>
       </c>
@@ -78690,8 +78738,32 @@
       <c r="O1">
         <v>54</v>
       </c>
+      <c r="Z1">
+        <v>5</v>
+      </c>
+      <c r="AA1">
+        <v>5</v>
+      </c>
+      <c r="AE1">
+        <v>12</v>
+      </c>
+      <c r="AF1">
+        <v>12</v>
+      </c>
+      <c r="AK1">
+        <v>7</v>
+      </c>
+      <c r="AL1">
+        <v>7</v>
+      </c>
+      <c r="AS1">
+        <v>41</v>
+      </c>
+      <c r="AT1">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -78719,8 +78791,38 @@
       <c r="V2" t="s">
         <v>621</v>
       </c>
+      <c r="Z2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>622</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>623</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -78751,8 +78853,32 @@
       <c r="S3" t="s">
         <v>19</v>
       </c>
+      <c r="Z3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AS3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AT3" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -78798,8 +78924,48 @@
         <f>STANDARDIZE(V4,$V$23,$V$24)</f>
         <v>-1.1514931229028054</v>
       </c>
+      <c r="Z4">
+        <v>2.2995031937544399E-2</v>
+      </c>
+      <c r="AA4">
+        <v>7.8825133116870005E-2</v>
+      </c>
+      <c r="AE4">
+        <v>5.25195173882186E-3</v>
+      </c>
+      <c r="AF4">
+        <v>-0.83401138656248397</v>
+      </c>
+      <c r="AH4">
+        <f>AE4/B4</f>
+        <v>5.3468208092485578E-2</v>
+      </c>
+      <c r="AI4">
+        <f>STANDARDIZE(AH4,$AH$23,$AH$24)</f>
+        <v>-1.0118146336877887</v>
+      </c>
+      <c r="AK4">
+        <v>2.3136976579134098E-2</v>
+      </c>
+      <c r="AL4">
+        <v>1.73282323878279</v>
+      </c>
+      <c r="AN4">
+        <f>AK4/B4</f>
+        <v>0.23554913294797658</v>
+      </c>
+      <c r="AO4">
+        <f>STANDARDIZE(AN4,$AN$23,$AN$24)</f>
+        <v>0.25104523176116372</v>
+      </c>
+      <c r="AS4">
+        <v>1.13555713271824E-3</v>
+      </c>
+      <c r="AT4">
+        <v>-0.477829865575293</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -78845,8 +79011,48 @@
         <f t="shared" ref="W5:W21" si="5">STANDARDIZE(V5,$V$23,$V$24)</f>
         <v>2.3172273662213967</v>
       </c>
+      <c r="Z5">
+        <v>1.0443864229764999E-2</v>
+      </c>
+      <c r="AA5">
+        <v>-0.78153514014362502</v>
+      </c>
+      <c r="AE5">
+        <v>2.34986945169713E-2</v>
+      </c>
+      <c r="AF5">
+        <v>2.0208183416382499</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" ref="AH5:AH21" si="6">AE5/B5</f>
+        <v>0.40909090909090923</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" ref="AI5:AI21" si="7">STANDARDIZE(AH5,$AH$23,$AH$24)</f>
+        <v>2.2416229014735767</v>
+      </c>
+      <c r="AK5">
+        <v>1.8276762402088802E-2</v>
+      </c>
+      <c r="AL5">
+        <v>0.70126190298593305</v>
+      </c>
+      <c r="AN5">
+        <f t="shared" ref="AN5:AN21" si="8">AK5/B5</f>
+        <v>0.31818181818181851</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" ref="AO5:AO21" si="9">STANDARDIZE(AN5,$AN$23,$AN$24)</f>
+        <v>1.7536490093835071</v>
+      </c>
+      <c r="AS5">
+        <v>1.3054830287206299E-3</v>
+      </c>
+      <c r="AT5">
+        <v>-0.42147371265460098</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -78892,8 +79098,48 @@
         <f t="shared" si="5"/>
         <v>1.2421529080950549</v>
       </c>
+      <c r="Z6">
+        <v>1.9547953573610301E-2</v>
+      </c>
+      <c r="AA6">
+        <v>-0.15746597159894801</v>
+      </c>
+      <c r="AE6">
+        <v>1.03848503359805E-2</v>
+      </c>
+      <c r="AF6">
+        <v>-3.09337257891911E-2</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" si="6"/>
+        <v>0.15887850467289796</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" si="7"/>
+        <v>-4.7461642373194383E-2</v>
+      </c>
+      <c r="AK6">
+        <v>1.6493585827733699E-2</v>
+      </c>
+      <c r="AL6">
+        <v>0.32278969126918999</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" si="8"/>
+        <v>0.25233644859813148</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" si="9"/>
+        <v>0.5563080202168238</v>
+      </c>
+      <c r="AS6">
+        <v>6.1087354917532105E-4</v>
+      </c>
+      <c r="AT6">
+        <v>-0.65184188472454596</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -78939,8 +79185,48 @@
         <f t="shared" si="5"/>
         <v>-0.26931272060801159</v>
       </c>
+      <c r="Z7">
+        <v>1.8181818181818198E-2</v>
+      </c>
+      <c r="AA7">
+        <v>-0.25111212838359198</v>
+      </c>
+      <c r="AE7">
+        <v>6.4935064935064896E-3</v>
+      </c>
+      <c r="AF7">
+        <v>-0.63976151599889297</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="6"/>
+        <v>8.875739644970404E-2</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="7"/>
+        <v>-0.6889691863515599</v>
+      </c>
+      <c r="AK7">
+        <v>1.6883116883116899E-2</v>
+      </c>
+      <c r="AL7">
+        <v>0.40546612510276198</v>
+      </c>
+      <c r="AN7">
+        <f t="shared" si="8"/>
+        <v>0.23076923076923087</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" si="9"/>
+        <v>0.16412685254931286</v>
+      </c>
+      <c r="AS7">
+        <v>2.8138528138528102E-3</v>
+      </c>
+      <c r="AT7">
+        <v>7.8779163873805805E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -78986,8 +79272,48 @@
         <f t="shared" si="5"/>
         <v>0.22212521775594285</v>
       </c>
+      <c r="Z8">
+        <v>1.98098256735341E-2</v>
+      </c>
+      <c r="AA8">
+        <v>-0.13951510386334201</v>
+      </c>
+      <c r="AE8">
+        <v>6.3391442155309001E-3</v>
+      </c>
+      <c r="AF8">
+        <v>-0.6639125672542</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="6"/>
+        <v>8.2474226804123682E-2</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="7"/>
+        <v>-0.74645117472667288</v>
+      </c>
+      <c r="AK8">
+        <v>1.42630744849445E-2</v>
+      </c>
+      <c r="AL8">
+        <v>-0.15062756493830801</v>
+      </c>
+      <c r="AN8">
+        <f t="shared" si="8"/>
+        <v>0.18556701030927794</v>
+      </c>
+      <c r="AO8">
+        <f t="shared" si="9"/>
+        <v>-0.65783635762392279</v>
+      </c>
+      <c r="AS8">
+        <v>7.9239302694136295E-4</v>
+      </c>
+      <c r="AT8">
+        <v>-0.59164070475299302</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -79033,8 +79359,48 @@
         <f t="shared" si="5"/>
         <v>-0.82160321811928461</v>
       </c>
+      <c r="Z9">
+        <v>3.4539115275659199E-2</v>
+      </c>
+      <c r="AA9">
+        <v>0.87015155999318405</v>
+      </c>
+      <c r="AE9">
+        <v>2.3697973414687299E-2</v>
+      </c>
+      <c r="AF9">
+        <v>2.0519969102364799</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="6"/>
+        <v>0.32608695652173908</v>
+      </c>
+      <c r="AI9">
+        <f t="shared" si="7"/>
+        <v>1.4822558135539312</v>
+      </c>
+      <c r="AK9">
+        <v>1.10590542601874E-2</v>
+      </c>
+      <c r="AL9">
+        <v>-0.83066825091891805</v>
+      </c>
+      <c r="AN9">
+        <f t="shared" si="8"/>
+        <v>0.15217391304347813</v>
+      </c>
+      <c r="AO9">
+        <f t="shared" si="9"/>
+        <v>-1.2650608954216065</v>
+      </c>
+      <c r="AS9">
+        <v>1.2421006755284399E-2</v>
+      </c>
+      <c r="AT9">
+        <v>3.2650047445136199</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -79080,8 +79446,48 @@
         <f t="shared" si="5"/>
         <v>0.79395976641955057</v>
       </c>
+      <c r="Z10">
+        <v>1.1264080100125201E-2</v>
+      </c>
+      <c r="AA10">
+        <v>-0.72531079777281504</v>
+      </c>
+      <c r="AE10">
+        <v>1.6270337922403001E-2</v>
+      </c>
+      <c r="AF10">
+        <v>0.88989171308289505</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="6"/>
+        <v>0.35616438356164343</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="7"/>
+        <v>1.7574211216683195</v>
+      </c>
+      <c r="AK10">
+        <v>9.3867334167709593E-3</v>
+      </c>
+      <c r="AL10">
+        <v>-1.18561176992333</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" si="8"/>
+        <v>0.20547945205479423</v>
+      </c>
+      <c r="AO10">
+        <f t="shared" si="9"/>
+        <v>-0.29574585912655843</v>
+      </c>
+      <c r="AS10">
+        <v>2.5031289111389198E-3</v>
+      </c>
+      <c r="AT10">
+        <v>-2.4272838142486399E-2</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -79127,8 +79533,48 @@
         <f t="shared" si="5"/>
         <v>1.1750560624814985</v>
       </c>
+      <c r="Z11">
+        <v>1.50406504065041E-2</v>
+      </c>
+      <c r="AA11">
+        <v>-0.46643360511370202</v>
+      </c>
+      <c r="AE11">
+        <v>6.0975609756097598E-3</v>
+      </c>
+      <c r="AF11">
+        <v>-0.70170994421880795</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="6"/>
+        <v>0.15957446808510664</v>
+      </c>
+      <c r="AI11">
+        <f t="shared" si="7"/>
+        <v>-4.1094575585777088E-2</v>
+      </c>
+      <c r="AK11">
+        <v>9.3495934959349596E-3</v>
+      </c>
+      <c r="AL11">
+        <v>-1.19349457198788</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="8"/>
+        <v>0.24468085106383003</v>
+      </c>
+      <c r="AO11">
+        <f t="shared" si="9"/>
+        <v>0.41709761282845897</v>
+      </c>
+      <c r="AS11">
+        <v>4.0650406504065002E-3</v>
+      </c>
+      <c r="AT11">
+        <v>0.493737299791707</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -79174,8 +79620,48 @@
         <f t="shared" si="5"/>
         <v>-0.41304898886664726</v>
       </c>
+      <c r="Z12">
+        <v>1.67253521126761E-2</v>
+      </c>
+      <c r="AA12">
+        <v>-0.35095029280116102</v>
+      </c>
+      <c r="AE12">
+        <v>8.3626760563380292E-3</v>
+      </c>
+      <c r="AF12">
+        <v>-0.34731694658184997</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="6"/>
+        <v>9.9476439790575924E-2</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="7"/>
+        <v>-0.59090531740195462</v>
+      </c>
+      <c r="AK12">
+        <v>2.1126760563380299E-2</v>
+      </c>
+      <c r="AL12">
+        <v>1.3061627989517399</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="8"/>
+        <v>0.25130890052356042</v>
+      </c>
+      <c r="AO12">
+        <f t="shared" si="9"/>
+        <v>0.5376229488776838</v>
+      </c>
+      <c r="AS12">
+        <v>1.76056338028169E-3</v>
+      </c>
+      <c r="AT12">
+        <v>-0.27054569940218098</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -79221,8 +79707,48 @@
         <f t="shared" si="5"/>
         <v>-0.34962688648023627</v>
       </c>
+      <c r="Z13">
+        <v>1.7925430210325E-2</v>
+      </c>
+      <c r="AA13">
+        <v>-0.26868706884732402</v>
+      </c>
+      <c r="AE13">
+        <v>1.4579349904397699E-2</v>
+      </c>
+      <c r="AF13">
+        <v>0.62532488477128501</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="6"/>
+        <v>0.21107266435986163</v>
+      </c>
+      <c r="AI13">
+        <f t="shared" si="7"/>
+        <v>0.4300400406324878</v>
+      </c>
+      <c r="AK13">
+        <v>1.4340344168259999E-2</v>
+      </c>
+      <c r="AL13">
+        <v>-0.13422737868437601</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="8"/>
+        <v>0.20761245674740442</v>
+      </c>
+      <c r="AO13">
+        <f t="shared" si="9"/>
+        <v>-0.25695901709507585</v>
+      </c>
+      <c r="AS13">
+        <v>4.5411089866156801E-3</v>
+      </c>
+      <c r="AT13">
+        <v>0.65162600650022895</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -79268,8 +79794,48 @@
         <f t="shared" si="5"/>
         <v>-0.46928549946879566</v>
       </c>
+      <c r="Z14">
+        <v>5.0944476244991398E-2</v>
+      </c>
+      <c r="AA14">
+        <v>1.99470994174147</v>
+      </c>
+      <c r="AE14">
+        <v>1.2020606754436201E-2</v>
+      </c>
+      <c r="AF14">
+        <v>0.224991734896027</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="6"/>
+        <v>0.13043478260869595</v>
+      </c>
+      <c r="AI14">
+        <f t="shared" si="7"/>
+        <v>-0.30768089368522611</v>
+      </c>
+      <c r="AK14">
+        <v>2.1751574127074999E-2</v>
+      </c>
+      <c r="AL14">
+        <v>1.4387770194181999</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" si="8"/>
+        <v>0.23602484472049709</v>
+      </c>
+      <c r="AO14">
+        <f t="shared" si="9"/>
+        <v>0.25969563812791691</v>
+      </c>
+      <c r="AS14">
+        <v>1.1448196908986799E-3</v>
+      </c>
+      <c r="AT14">
+        <v>-0.47475792564421498</v>
+      </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -79315,8 +79881,48 @@
         <f t="shared" si="5"/>
         <v>0.49130725480047083</v>
       </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>-1.49744349957435</v>
+      </c>
+      <c r="AE15">
+        <v>1.7391304347826101E-2</v>
+      </c>
+      <c r="AF15">
+        <v>1.0652747014069801</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="6"/>
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" si="7"/>
+        <v>1.1129037945998215</v>
+      </c>
+      <c r="AK15">
+        <v>8.6956521739130401E-3</v>
+      </c>
+      <c r="AL15">
+        <v>-1.3322910445515199</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="8"/>
+        <v>0.14285714285714282</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="9"/>
+        <v>-1.4344782880382176</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15">
+        <v>-0.85443892238881503</v>
+      </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -79362,8 +79968,48 @@
         <f t="shared" si="5"/>
         <v>1.0135204066668573</v>
       </c>
+      <c r="Z16">
+        <v>1.30796670630202E-2</v>
+      </c>
+      <c r="AA16">
+        <v>-0.600855533378857</v>
+      </c>
+      <c r="AE16">
+        <v>7.72889417360285E-3</v>
+      </c>
+      <c r="AF16">
+        <v>-0.446476527117731</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" si="6"/>
+        <v>0.13</v>
+      </c>
+      <c r="AI16">
+        <f t="shared" si="7"/>
+        <v>-0.311658530812427</v>
+      </c>
+      <c r="AK16">
+        <v>1.12960760998811E-2</v>
+      </c>
+      <c r="AL16">
+        <v>-0.78036129804383103</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" si="8"/>
+        <v>0.19000000000000022</v>
+      </c>
+      <c r="AO16">
+        <f t="shared" si="9"/>
+        <v>-0.57722628139815102</v>
+      </c>
+      <c r="AS16">
+        <v>0</v>
+      </c>
+      <c r="AT16">
+        <v>-0.85443892238881503</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -79409,8 +80055,48 @@
         <f t="shared" si="5"/>
         <v>-0.14295973127206171</v>
       </c>
+      <c r="Z17">
+        <v>5.3634438955539897E-2</v>
+      </c>
+      <c r="AA17">
+        <v>2.1791021119834202</v>
+      </c>
+      <c r="AE17">
+        <v>3.8108680310515201E-3</v>
+      </c>
+      <c r="AF17">
+        <v>-1.0594789486248499</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" si="6"/>
+        <v>6.7669172932330837E-2</v>
+      </c>
+      <c r="AI17">
+        <f t="shared" si="7"/>
+        <v>-0.88189617821307986</v>
+      </c>
+      <c r="AK17">
+        <v>9.5977417078334498E-3</v>
+      </c>
+      <c r="AL17">
+        <v>-1.1408260903907901</v>
+      </c>
+      <c r="AN17">
+        <f t="shared" si="8"/>
+        <v>0.17042606516290715</v>
+      </c>
+      <c r="AO17">
+        <f t="shared" si="9"/>
+        <v>-0.93316132509081462</v>
+      </c>
+      <c r="AS17">
+        <v>3.6697247706421999E-3</v>
+      </c>
+      <c r="AT17">
+        <v>0.36263025433195001</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -79456,8 +80142,48 @@
         <f t="shared" si="5"/>
         <v>-0.25317279062903925</v>
       </c>
+      <c r="Z18">
+        <v>1.9129019129019102E-2</v>
+      </c>
+      <c r="AA18">
+        <v>-0.18618318434109499</v>
+      </c>
+      <c r="AE18">
+        <v>5.1553384886718198E-3</v>
+      </c>
+      <c r="AF18">
+        <v>-0.84912720104071004</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="6"/>
+        <v>5.9936908517350097E-2</v>
+      </c>
+      <c r="AI18">
+        <f t="shared" si="7"/>
+        <v>-0.95263530484606274</v>
+      </c>
+      <c r="AK18">
+        <v>1.9671686338352999E-2</v>
+      </c>
+      <c r="AL18">
+        <v>0.99732901990926903</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" si="8"/>
+        <v>0.22870662460567803</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" si="9"/>
+        <v>0.12662014676659536</v>
+      </c>
+      <c r="AS18">
+        <v>1.89933523266857E-3</v>
+      </c>
+      <c r="AT18">
+        <v>-0.224521827124982</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -79503,8 +80229,48 @@
         <f t="shared" si="5"/>
         <v>-0.78998496131731499</v>
       </c>
+      <c r="Z19">
+        <v>1.5424164524421601E-2</v>
+      </c>
+      <c r="AA19">
+        <v>-0.44014439290866803</v>
+      </c>
+      <c r="AE19">
+        <v>4.71293916023993E-3</v>
+      </c>
+      <c r="AF19">
+        <v>-0.91834365078733704</v>
+      </c>
+      <c r="AH19">
+        <f t="shared" si="6"/>
+        <v>9.4827586206896547E-2</v>
+      </c>
+      <c r="AI19">
+        <f t="shared" si="7"/>
+        <v>-0.63343565841266236</v>
+      </c>
+      <c r="AK19">
+        <v>1.19965724078835E-2</v>
+      </c>
+      <c r="AL19">
+        <v>-0.63168371288379199</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="8"/>
+        <v>0.24137931034482843</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" si="9"/>
+        <v>0.35706195572368332</v>
+      </c>
+      <c r="AS19">
+        <v>1.2853470437018E-3</v>
+      </c>
+      <c r="AT19">
+        <v>-0.42815183928289202</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -79550,8 +80316,48 @@
         <f t="shared" si="5"/>
         <v>-1.5172048677625456</v>
       </c>
+      <c r="Z20">
+        <v>1.01744186046512E-2</v>
+      </c>
+      <c r="AA20">
+        <v>-0.80000515959114804</v>
+      </c>
+      <c r="AE20">
+        <v>4.3604651162790697E-3</v>
+      </c>
+      <c r="AF20">
+        <v>-0.97349066476966795</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="6"/>
+        <v>8.1081081081081016E-2</v>
+      </c>
+      <c r="AI20">
+        <f t="shared" si="7"/>
+        <v>-0.75919645947528802</v>
+      </c>
+      <c r="AK20">
+        <v>1.8895348837209301E-2</v>
+      </c>
+      <c r="AL20">
+        <v>0.83255443991414502</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="8"/>
+        <v>0.35135135135135109</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" si="9"/>
+        <v>2.3568082278146325</v>
+      </c>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+      <c r="AT20">
+        <v>-0.85443892238881503</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -79597,8 +80403,48 @@
         <f t="shared" si="5"/>
         <v>-1.0776561950140306</v>
       </c>
+      <c r="Z21">
+        <v>4.4352667229966398E-2</v>
+      </c>
+      <c r="AA21">
+        <v>1.54285313148367</v>
+      </c>
+      <c r="AE21">
+        <v>1.4329695977362E-2</v>
+      </c>
+      <c r="AF21">
+        <v>0.58626479271380705</v>
+      </c>
+      <c r="AH21">
+        <f t="shared" si="6"/>
+        <v>0.15848691606533732</v>
+      </c>
+      <c r="AI21">
+        <f t="shared" si="7"/>
+        <v>-5.1044116356442723E-2</v>
+      </c>
+      <c r="AK21">
+        <v>1.3288992874809899E-2</v>
+      </c>
+      <c r="AL21">
+        <v>-0.35737255401129397</v>
+      </c>
+      <c r="AN21">
+        <f t="shared" si="8"/>
+        <v>0.14697670499570409</v>
+      </c>
+      <c r="AO21">
+        <f t="shared" si="9"/>
+        <v>-1.3595676202554283</v>
+      </c>
+      <c r="AS21">
+        <v>6.4254661216678497E-3</v>
+      </c>
+      <c r="AT21">
+        <v>1.2765755954593201</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>617</v>
       </c>
@@ -79607,15 +80453,15 @@
         <v>6.8303546248804123E-2</v>
       </c>
       <c r="F23">
-        <f t="shared" ref="F23:N23" si="6">AVERAGE(F4:F21)</f>
+        <f t="shared" ref="F23:N23" si="10">AVERAGE(F4:F21)</f>
         <v>1.2947623272551849E-2</v>
       </c>
       <c r="I23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>0.19191465808413349</v>
       </c>
       <c r="N23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="10"/>
         <v>2.2724578927246363E-3</v>
       </c>
       <c r="R23">
@@ -79626,8 +80472,16 @@
         <f>AVERAGE(V4:V21)</f>
         <v>3.5970831360301499E-2</v>
       </c>
+      <c r="AH23">
+        <f>AVERAGE(AH4:AH21)</f>
+        <v>0.16406638280861249</v>
+      </c>
+      <c r="AN23">
+        <f>AVERAGE(AN4:AN21)</f>
+        <v>0.22174340323764508</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>618</v>
       </c>
@@ -79636,15 +80490,15 @@
         <v>1.7167314127054238E-2</v>
       </c>
       <c r="F24">
-        <f t="shared" ref="F24:N24" si="7">_xlfn.STDEV.S(F4:F21)</f>
+        <f t="shared" ref="F24:N24" si="11">_xlfn.STDEV.S(F4:F21)</f>
         <v>5.035907380167591E-3</v>
       </c>
       <c r="I24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>6.5045311725725655E-2</v>
       </c>
       <c r="N24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="11"/>
         <v>1.2881614965945898E-3</v>
       </c>
       <c r="R24">
@@ -79655,9 +80509,18 @@
         <f>_xlfn.STDEV.S(V4:V21)</f>
         <v>2.3708618476388395E-2</v>
       </c>
+      <c r="AH24">
+        <f>_xlfn.STDEV.S(AH4:AH21)</f>
+        <v>0.10930675544099092</v>
+      </c>
+      <c r="AN24">
+        <f>_xlfn.STDEV.S(AN4:AN21)</f>
+        <v>5.4992997132348752E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -79665,16 +80528,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>1</v>
       </c>
@@ -79694,7 +80557,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>20</v>
       </c>
@@ -79714,7 +80577,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -79734,7 +80597,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -79757,7 +80620,7 @@
         <v>0.49471025533581803</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -79780,7 +80643,7 @@
         <v>0.23580062580990899</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -79803,7 +80666,7 @@
         <v>-0.87979167193233299</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -79826,7 +80689,7 @@
         <v>0.95020583911318701</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -79849,7 +80712,7 @@
         <v>-6.0522362531776799E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -79872,7 +80735,7 @@
         <v>-0.86395968446069304</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -79895,7 +80758,7 @@
         <v>-0.82625124205842504</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -79918,7 +80781,7 @@
         <v>-0.66912118580433899</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -79941,7 +80804,7 @@
         <v>0.73856764132767105</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -79964,7 +80827,7 @@
         <v>0.81412429129669905</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -79987,7 +80850,7 @@
         <v>7.0363343258534203E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -80010,7 +80873,7 @@
         <v>1.8249411226654699</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -80033,7 +80896,7 @@
         <v>0.94542131794274598</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -80056,7 +80919,7 @@
         <v>-2.2089034153531699</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -80079,7 +80942,7 @@
         <v>1.0820391624747701</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -80102,7 +80965,7 @@
         <v>9.4247007020184195E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -80125,7 +80988,7 @@
         <v>-0.61719773292643398</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -80148,7 +81011,7 @@
         <v>-1.12467331117782</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>617</v>
       </c>
@@ -80157,13 +81020,1404 @@
         <v>6.8303546248804123E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>618</v>
       </c>
       <c r="B24">
         <f>_xlfn.STDEV.S(B4:B21)</f>
         <v>1.7167314127054238E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>10</v>
+      </c>
+      <c r="N1">
+        <v>20</v>
+      </c>
+      <c r="O1">
+        <v>20</v>
+      </c>
+      <c r="Q1">
+        <v>4</v>
+      </c>
+      <c r="R1">
+        <v>4</v>
+      </c>
+      <c r="AB1">
+        <v>107</v>
+      </c>
+      <c r="AC1">
+        <v>107</v>
+      </c>
+      <c r="AE1">
+        <v>7</v>
+      </c>
+      <c r="AF1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" t="s">
+        <v>628</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
+        <v>23</v>
+      </c>
+      <c r="T2" t="s">
+        <v>625</v>
+      </c>
+      <c r="W2" t="s">
+        <v>624</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>19</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>9.8225691980127705E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.7429718772471701</v>
+      </c>
+      <c r="E4">
+        <v>1.6891412349183801E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.49471025533581803</v>
+      </c>
+      <c r="H4">
+        <f>E4/B4</f>
+        <v>0.17196531791907504</v>
+      </c>
+      <c r="I4">
+        <f>STANDARDIZE(H4,$H$23,$H$24)</f>
+        <v>-0.62434044742169104</v>
+      </c>
+      <c r="N4">
+        <v>6.9552874378992196E-3</v>
+      </c>
+      <c r="O4">
+        <v>4.2498527527714901E-2</v>
+      </c>
+      <c r="Q4">
+        <v>4.01703335699077E-2</v>
+      </c>
+      <c r="R4">
+        <v>0.95066893797460095</v>
+      </c>
+      <c r="T4">
+        <f>N4/Q4</f>
+        <v>0.17314487632508851</v>
+      </c>
+      <c r="U4">
+        <f>STANDARDIZE(T4,$T$23,$T$24)</f>
+        <v>-0.61270332025513141</v>
+      </c>
+      <c r="W4">
+        <f>N4/B4</f>
+        <v>7.0809248554913329E-2</v>
+      </c>
+      <c r="X4">
+        <f>STANDARDIZE(W4,$W$23,$W$24)</f>
+        <v>-0.58495331996239841</v>
+      </c>
+      <c r="AB4">
+        <v>7.0972320794889996E-4</v>
+      </c>
+      <c r="AC4">
+        <v>-0.427998060596123</v>
+      </c>
+      <c r="AE4">
+        <v>2.3136976579134098E-2</v>
+      </c>
+      <c r="AF4">
+        <v>1.73282323878279</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>5.7441253263707602E-2</v>
+      </c>
+      <c r="C5">
+        <v>-0.63273106699774695</v>
+      </c>
+      <c r="E5">
+        <v>1.5665796344647501E-2</v>
+      </c>
+      <c r="F5">
+        <v>0.23580062580990899</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H21" si="0">E5/B5</f>
+        <v>0.27272727272727226</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ref="I5:I21" si="1">STANDARDIZE(H5,$H$23,$H$24)</f>
+        <v>0.64272740200714407</v>
+      </c>
+      <c r="N5">
+        <v>5.2219321148825101E-3</v>
+      </c>
+      <c r="O5">
+        <v>-0.46304911890287098</v>
+      </c>
+      <c r="Q5">
+        <v>2.2193211488250601E-2</v>
+      </c>
+      <c r="R5">
+        <v>-0.51343672800482099</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ref="T5:T21" si="2">N5/Q5</f>
+        <v>0.23529411764705954</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ref="U5:U21" si="3">STANDARDIZE(T5,$T$23,$T$24)</f>
+        <v>-0.23188184724587116</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ref="W5:W21" si="4">N5/B5</f>
+        <v>9.0909090909090925E-2</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ref="X5:X21" si="5">STANDARDIZE(W5,$W$23,$W$24)</f>
+        <v>-0.26001039623428157</v>
+      </c>
+      <c r="AB5">
+        <v>1.3054830287206299E-3</v>
+      </c>
+      <c r="AC5">
+        <v>0.35566022448053702</v>
+      </c>
+      <c r="AE5">
+        <v>1.8276762402088802E-2</v>
+      </c>
+      <c r="AF5">
+        <v>0.70126190298593305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>6.5363469761759302E-2</v>
+      </c>
+      <c r="C6">
+        <v>-0.17126013220737199</v>
+      </c>
+      <c r="E6">
+        <v>1.03848503359805E-2</v>
+      </c>
+      <c r="F6">
+        <v>-0.87979167193233299</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0.15887850467289796</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>-0.78890534046365701</v>
+      </c>
+      <c r="N6">
+        <v>7.9413561392791699E-3</v>
+      </c>
+      <c r="O6">
+        <v>0.33009375083940501</v>
+      </c>
+      <c r="Q6">
+        <v>2.3213194868662201E-2</v>
+      </c>
+      <c r="R6">
+        <v>-0.43036651022012201</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="2"/>
+        <v>0.34210526315789458</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="3"/>
+        <v>0.4226068786344051</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="4"/>
+        <v>0.12149532710280378</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="5"/>
+        <v>0.23446019908151217</v>
+      </c>
+      <c r="AB6">
+        <v>1.2217470983506399E-3</v>
+      </c>
+      <c r="AC6">
+        <v>0.24551456962915899</v>
+      </c>
+      <c r="AE6">
+        <v>1.6493585827733699E-2</v>
+      </c>
+      <c r="AF6">
+        <v>0.32278969126918999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>7.3160173160173203E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.28289963563463999</v>
+      </c>
+      <c r="E7">
+        <v>1.9047619047619001E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.95020583911318701</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0.26035502958579804</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0.48714813064704648</v>
+      </c>
+      <c r="N7">
+        <v>3.8961038961039E-3</v>
+      </c>
+      <c r="O7">
+        <v>-0.84973806067636404</v>
+      </c>
+      <c r="Q7">
+        <v>2.4891774891774899E-2</v>
+      </c>
+      <c r="R7">
+        <v>-0.29365839245377501</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="2"/>
+        <v>0.15652173913043491</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="3"/>
+        <v>-0.71456212750440129</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="4"/>
+        <v>5.3254437869822507E-2</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="5"/>
+        <v>-0.86875213833081211</v>
+      </c>
+      <c r="AB7">
+        <v>6.4935064935064902E-4</v>
+      </c>
+      <c r="AC7">
+        <v>-0.50741170026640103</v>
+      </c>
+      <c r="AE7">
+        <v>1.6883116883116899E-2</v>
+      </c>
+      <c r="AF7">
+        <v>0.40546612510276198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>7.6862123613312197E-2</v>
+      </c>
+      <c r="C8">
+        <v>0.498539101758526</v>
+      </c>
+      <c r="E8">
+        <v>1.42630744849445E-2</v>
+      </c>
+      <c r="F8">
+        <v>-6.0522362531776799E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0.18556701030927794</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>-0.45330101931360428</v>
+      </c>
+      <c r="N8">
+        <v>1.10935023771791E-2</v>
+      </c>
+      <c r="O8">
+        <v>1.24944369058627</v>
+      </c>
+      <c r="Q8">
+        <v>3.0110935023771799E-2</v>
+      </c>
+      <c r="R8">
+        <v>0.131404189098556</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="2"/>
+        <v>0.36842105263157948</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="3"/>
+        <v>0.58385772414114545</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="4"/>
+        <v>0.14432989690721676</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="5"/>
+        <v>0.60361393390060891</v>
+      </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8">
+        <v>-1.3615629849642701</v>
+      </c>
+      <c r="AE8">
+        <v>1.42630744849445E-2</v>
+      </c>
+      <c r="AF8">
+        <v>-0.15062756493830801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>7.26737851383744E-2</v>
+      </c>
+      <c r="C9">
+        <v>0.25456742139314198</v>
+      </c>
+      <c r="E9">
+        <v>1.0459795162344699E-2</v>
+      </c>
+      <c r="F9">
+        <v>-0.86395968446069304</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0.14392803598200843</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>-0.9769054467356868</v>
+      </c>
+      <c r="N9">
+        <v>3.97690128568316E-3</v>
+      </c>
+      <c r="O9">
+        <v>-0.82617282301439399</v>
+      </c>
+      <c r="Q9">
+        <v>3.0943560688603201E-2</v>
+      </c>
+      <c r="R9">
+        <v>0.19921548547748899</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="2"/>
+        <v>0.12852112676056346</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="3"/>
+        <v>-0.88613677943963076</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="4"/>
+        <v>5.4722638680659713E-2</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="5"/>
+        <v>-0.84501655594728775</v>
+      </c>
+      <c r="AB9">
+        <v>1.6888210939202399E-3</v>
+      </c>
+      <c r="AC9">
+        <v>0.85990042381086595</v>
+      </c>
+      <c r="AE9">
+        <v>1.10590542601874E-2</v>
+      </c>
+      <c r="AF9">
+        <v>-0.83066825091891805</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>4.5682102628285398E-2</v>
+      </c>
+      <c r="C10">
+        <v>-1.3177042985931799</v>
+      </c>
+      <c r="E10">
+        <v>1.0638297872340399E-2</v>
+      </c>
+      <c r="F10">
+        <v>-0.82625124205842504</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0.23287671232876633</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.14161203600631436</v>
+      </c>
+      <c r="N10">
+        <v>5.6320400500625804E-3</v>
+      </c>
+      <c r="O10">
+        <v>-0.34343769321320999</v>
+      </c>
+      <c r="Q10">
+        <v>1.6270337922403001E-2</v>
+      </c>
+      <c r="R10">
+        <v>-0.99581164359186303</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="2"/>
+        <v>0.34615384615384637</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="3"/>
+        <v>0.44741470102005909</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="4"/>
+        <v>0.12328767123287665</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="5"/>
+        <v>0.26343602544324268</v>
+      </c>
+      <c r="AB10">
+        <v>1.2515644555694599E-3</v>
+      </c>
+      <c r="AC10">
+        <v>0.28473611195027498</v>
+      </c>
+      <c r="AE10">
+        <v>9.3867334167709593E-3</v>
+      </c>
+      <c r="AF10">
+        <v>-1.18561176992333</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>3.82113821138211E-2</v>
+      </c>
+      <c r="C11">
+        <v>-1.7528754884003801</v>
+      </c>
+      <c r="E11">
+        <v>1.13821138211382E-2</v>
+      </c>
+      <c r="F11">
+        <v>-0.66912118580433899</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0.2978723404255319</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0.95892320143187271</v>
+      </c>
+      <c r="N11">
+        <v>7.3170731707317103E-3</v>
+      </c>
+      <c r="O11">
+        <v>0.14801637682090699</v>
+      </c>
+      <c r="Q11">
+        <v>1.6666666666666701E-2</v>
+      </c>
+      <c r="R11">
+        <v>-0.96353355383805295</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="2"/>
+        <v>0.43902439024390172</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="3"/>
+        <v>1.0164819437933563</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="4"/>
+        <v>0.19148936170212794</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="5"/>
+        <v>1.3660146583384616</v>
+      </c>
+      <c r="AB11">
+        <v>4.0650406504065003E-4</v>
+      </c>
+      <c r="AC11">
+        <v>-0.82685039210462996</v>
+      </c>
+      <c r="AE11">
+        <v>9.3495934959349596E-3</v>
+      </c>
+      <c r="AF11">
+        <v>-1.19349457198788</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>8.4066901408450703E-2</v>
+      </c>
+      <c r="C12">
+        <v>0.91821906694215205</v>
+      </c>
+      <c r="E12">
+        <v>1.80457746478873E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.73856764132767105</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>0.21465968586387407</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>-8.7464589092878534E-2</v>
+      </c>
+      <c r="N12">
+        <v>9.2429577464788696E-3</v>
+      </c>
+      <c r="O12">
+        <v>0.70971679775448604</v>
+      </c>
+      <c r="Q12">
+        <v>3.60915492957746E-2</v>
+      </c>
+      <c r="R12">
+        <v>0.61848166467576204</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="2"/>
+        <v>0.25609756097560998</v>
+      </c>
+      <c r="U12">
+        <f t="shared" si="3"/>
+        <v>-0.10440807985102256</v>
+      </c>
+      <c r="W12">
+        <f t="shared" si="4"/>
+        <v>0.10994764397905755</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="5"/>
+        <v>4.7775256463739021E-2</v>
+      </c>
+      <c r="AB12">
+        <v>8.8028169014084498E-4</v>
+      </c>
+      <c r="AC12">
+        <v>-0.20364663070835501</v>
+      </c>
+      <c r="AE12">
+        <v>2.1126760563380299E-2</v>
+      </c>
+      <c r="AF12">
+        <v>1.3061627989517399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>6.9072657743785806E-2</v>
+      </c>
+      <c r="C13">
+        <v>4.4800921640367898E-2</v>
+      </c>
+      <c r="E13">
+        <v>1.8403441682600399E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.81412429129669905</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0.26643598615916997</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0.56361533081757842</v>
+      </c>
+      <c r="N13">
+        <v>2.62906309751434E-3</v>
+      </c>
+      <c r="O13">
+        <v>-1.21928115732413</v>
+      </c>
+      <c r="Q13">
+        <v>2.77246653919694E-2</v>
+      </c>
+      <c r="R13">
+        <v>-6.2940093184610593E-2</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>9.4827586206896561E-2</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="3"/>
+        <v>-1.0925950317306137</v>
+      </c>
+      <c r="W13">
+        <f t="shared" si="4"/>
+        <v>3.8062283737024243E-2</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="5"/>
+        <v>-1.1143552079794468</v>
+      </c>
+      <c r="AB13">
+        <v>2.15105162523901E-3</v>
+      </c>
+      <c r="AC13">
+        <v>1.4679152191257201</v>
+      </c>
+      <c r="AE13">
+        <v>1.4340344168259999E-2</v>
+      </c>
+      <c r="AF13">
+        <v>-0.13422737868437601</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>9.2157985117343993E-2</v>
+      </c>
+      <c r="C14">
+        <v>1.3895265556390799</v>
+      </c>
+      <c r="E14">
+        <v>1.48826559816829E-2</v>
+      </c>
+      <c r="F14">
+        <v>7.0363343258534203E-2</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>0.16149068322981386</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>-0.75605755110967077</v>
+      </c>
+      <c r="N14">
+        <v>6.8689181453921002E-3</v>
+      </c>
+      <c r="O14">
+        <v>1.7308197552637301E-2</v>
+      </c>
+      <c r="Q14">
+        <v>3.7206639954207199E-2</v>
+      </c>
+      <c r="R14">
+        <v>0.70929767758795503</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="2"/>
+        <v>0.18461538461538465</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="3"/>
+        <v>-0.54241741216744488</v>
+      </c>
+      <c r="W14">
+        <f t="shared" si="4"/>
+        <v>7.4534161490683246E-2</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="5"/>
+        <v>-0.52473473323650843</v>
+      </c>
+      <c r="AB14">
+        <v>5.7240984544934201E-4</v>
+      </c>
+      <c r="AC14">
+        <v>-0.60861909347330501</v>
+      </c>
+      <c r="AE14">
+        <v>2.1751574127074999E-2</v>
+      </c>
+      <c r="AF14">
+        <v>1.4387770194181999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>6.08695652173913E-2</v>
+      </c>
+      <c r="C15">
+        <v>-0.43303110646163701</v>
+      </c>
+      <c r="E15">
+        <v>2.3188405797101401E-2</v>
+      </c>
+      <c r="F15">
+        <v>1.8249411226654699</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>0.38095238095238021</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>2.0036433885421205</v>
+      </c>
+      <c r="N15">
+        <v>1.7391304347826101E-2</v>
+      </c>
+      <c r="O15">
+        <v>3.0862505597083998</v>
+      </c>
+      <c r="Q15">
+        <v>2.3188405797101401E-2</v>
+      </c>
+      <c r="R15">
+        <v>-0.43238539955967198</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="2"/>
+        <v>0.75000000000000222</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="3"/>
+        <v>2.9219949839888284</v>
+      </c>
+      <c r="W15">
+        <f t="shared" si="4"/>
+        <v>0.28571428571428598</v>
+      </c>
+      <c r="X15">
+        <f t="shared" si="5"/>
+        <v>2.8892963715508349</v>
+      </c>
+      <c r="AB15">
+        <v>2.8985507246376799E-3</v>
+      </c>
+      <c r="AC15">
+        <v>2.45117028586102</v>
+      </c>
+      <c r="AE15">
+        <v>8.6956521739130401E-3</v>
+      </c>
+      <c r="AF15">
+        <v>-1.3322910445515199</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>5.9453032104637302E-2</v>
+      </c>
+      <c r="C16">
+        <v>-0.51554448638060901</v>
+      </c>
+      <c r="E16">
+        <v>1.9024970273483901E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.94542131794274598</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>0.3199999999999994</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="1"/>
+        <v>1.2371755049256217</v>
+      </c>
+      <c r="N16">
+        <v>2.97265160523187E-3</v>
+      </c>
+      <c r="O16">
+        <v>-1.1190706816584199</v>
+      </c>
+      <c r="Q16">
+        <v>1.9619500594530302E-2</v>
+      </c>
+      <c r="R16">
+        <v>-0.72304673593449698</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="2"/>
+        <v>0.15151515151515182</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="3"/>
+        <v>-0.74524015397498344</v>
+      </c>
+      <c r="W16">
+        <f t="shared" si="4"/>
+        <v>5.0000000000000086E-2</v>
+      </c>
+      <c r="X16">
+        <f t="shared" si="5"/>
+        <v>-0.92136481746915411</v>
+      </c>
+      <c r="AB16">
+        <v>1.7835909631391199E-3</v>
+      </c>
+      <c r="AC16">
+        <v>0.98456004434855304</v>
+      </c>
+      <c r="AE16">
+        <v>1.12960760998811E-2</v>
+      </c>
+      <c r="AF16">
+        <v>-0.78036129804383103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>5.6316160903316898E-2</v>
+      </c>
+      <c r="C17">
+        <v>-0.698267955998784</v>
+      </c>
+      <c r="E17">
+        <v>4.0931545518701502E-3</v>
+      </c>
+      <c r="F17">
+        <v>-2.2089034153531699</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>7.2681704260651625E-2</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="1"/>
+        <v>-1.872818358366982</v>
+      </c>
+      <c r="N17">
+        <v>6.7748764996471396E-3</v>
+      </c>
+      <c r="O17">
+        <v>-1.0119838719856699E-2</v>
+      </c>
+      <c r="Q17">
+        <v>1.8772053634439002E-2</v>
+      </c>
+      <c r="R17">
+        <v>-0.79206511886870501</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="2"/>
+        <v>0.36090225563909673</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="3"/>
+        <v>0.53778605399635415</v>
+      </c>
+      <c r="W17">
+        <f t="shared" si="4"/>
+        <v>0.12030075187969914</v>
+      </c>
+      <c r="X17">
+        <f t="shared" si="5"/>
+        <v>0.21514816872978607</v>
+      </c>
+      <c r="AB17">
+        <v>1.41143260409315E-4</v>
+      </c>
+      <c r="AC17">
+        <v>-1.1759041312684799</v>
+      </c>
+      <c r="AE17">
+        <v>9.5977417078334498E-3</v>
+      </c>
+      <c r="AF17">
+        <v>-1.1408260903907901</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>8.6012752679419394E-2</v>
+      </c>
+      <c r="C18">
+        <v>1.0315653514318199</v>
+      </c>
+      <c r="E18">
+        <v>1.9671686338352999E-2</v>
+      </c>
+      <c r="F18">
+        <v>1.0820391624747701</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>0.22870662460567803</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="1"/>
+        <v>8.9173751206452254E-2</v>
+      </c>
+      <c r="N18">
+        <v>6.2406729073395699E-3</v>
+      </c>
+      <c r="O18">
+        <v>-0.165924805664451</v>
+      </c>
+      <c r="Q18">
+        <v>3.69013702347036E-2</v>
+      </c>
+      <c r="R18">
+        <v>0.68443568221700002</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="2"/>
+        <v>0.16911764705882326</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="3"/>
+        <v>-0.6373802969760517</v>
+      </c>
+      <c r="W18">
+        <f t="shared" si="4"/>
+        <v>7.2555205047318522E-2</v>
+      </c>
+      <c r="X18">
+        <f t="shared" si="5"/>
+        <v>-0.55672741662707625</v>
+      </c>
+      <c r="AB18">
+        <v>2.7133360466693801E-4</v>
+      </c>
+      <c r="AC18">
+        <v>-1.0046526665719999</v>
+      </c>
+      <c r="AE18">
+        <v>1.9671686338352999E-2</v>
+      </c>
+      <c r="AF18">
+        <v>0.99732901990926903</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>4.97000856898029E-2</v>
+      </c>
+      <c r="C19">
+        <v>-1.08365586027716</v>
+      </c>
+      <c r="E19">
+        <v>1.4995715509854299E-2</v>
+      </c>
+      <c r="F19">
+        <v>9.4247007020184195E-2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>0.30172413793103398</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="1"/>
+        <v>1.0073590301235846</v>
+      </c>
+      <c r="N19">
+        <v>7.2836332476435301E-3</v>
+      </c>
+      <c r="O19">
+        <v>0.13826334223557701</v>
+      </c>
+      <c r="Q19">
+        <v>1.9708654670094299E-2</v>
+      </c>
+      <c r="R19">
+        <v>-0.71578578578989605</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="2"/>
+        <v>0.3695652173913036</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="3"/>
+        <v>0.59086863046751736</v>
+      </c>
+      <c r="W19">
+        <f t="shared" si="4"/>
+        <v>0.14655172413793108</v>
+      </c>
+      <c r="X19">
+        <f t="shared" si="5"/>
+        <v>0.63953297364456996</v>
+      </c>
+      <c r="AB19">
+        <v>8.5689802913453304E-4</v>
+      </c>
+      <c r="AC19">
+        <v>-0.234405334206155</v>
+      </c>
+      <c r="AE19">
+        <v>1.19965724078835E-2</v>
+      </c>
+      <c r="AF19">
+        <v>-0.63168371288379199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>5.37790697674419E-2</v>
+      </c>
+      <c r="C20">
+        <v>-0.84605409872898396</v>
+      </c>
+      <c r="E20">
+        <v>1.16279069767442E-2</v>
+      </c>
+      <c r="F20">
+        <v>-0.61719773292643398</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>0.21621621621621631</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="1"/>
+        <v>-6.7891432043006156E-2</v>
+      </c>
+      <c r="N20">
+        <v>7.2674418604651196E-3</v>
+      </c>
+      <c r="O20">
+        <v>0.13354098809860299</v>
+      </c>
+      <c r="Q20">
+        <v>2.1802325581395301E-2</v>
+      </c>
+      <c r="R20">
+        <v>-0.54527153829196395</v>
+      </c>
+      <c r="T20">
+        <f t="shared" si="2"/>
+        <v>0.3333333333333342</v>
+      </c>
+      <c r="U20">
+        <f t="shared" si="3"/>
+        <v>0.3688565967988327</v>
+      </c>
+      <c r="W20">
+        <f t="shared" si="4"/>
+        <v>0.13513513513513509</v>
+      </c>
+      <c r="X20">
+        <f t="shared" si="5"/>
+        <v>0.45496735645206721</v>
+      </c>
+      <c r="AB20">
+        <v>1.45348837209302E-3</v>
+      </c>
+      <c r="AC20">
+        <v>0.55034541392340697</v>
+      </c>
+      <c r="AE20">
+        <v>1.8895348837209301E-2</v>
+      </c>
+      <c r="AF20">
+        <v>0.83255443991414502</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>9.0415640187322996E-2</v>
+      </c>
+      <c r="C21">
+        <v>1.28803456235895</v>
+      </c>
+      <c r="E21">
+        <v>9.2256394683664106E-3</v>
+      </c>
+      <c r="F21">
+        <v>-1.12467331117782</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>0.10203588062035222</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="1"/>
+        <v>-1.5036935911605522</v>
+      </c>
+      <c r="N21">
+        <v>3.8666173763706002E-3</v>
+      </c>
+      <c r="O21">
+        <v>-0.85833805195031099</v>
+      </c>
+      <c r="Q21">
+        <v>6.7479453488178798E-2</v>
+      </c>
+      <c r="R21">
+        <v>3.1747978627066198</v>
+      </c>
+      <c r="T21">
+        <f t="shared" si="2"/>
+        <v>5.730066229786468E-2</v>
+      </c>
+      <c r="U21">
+        <f t="shared" si="3"/>
+        <v>-1.3225424636953507</v>
+      </c>
+      <c r="W21">
+        <f t="shared" si="4"/>
+        <v>4.2764917312532964E-2</v>
+      </c>
+      <c r="X21">
+        <f t="shared" si="5"/>
+        <v>-1.0383303578178631</v>
+      </c>
+      <c r="AB21">
+        <v>3.8985435866070598E-4</v>
+      </c>
+      <c r="AC21">
+        <v>-0.84875129896980905</v>
+      </c>
+      <c r="AE21">
+        <v>1.3288992874809899E-2</v>
+      </c>
+      <c r="AF21">
+        <v>-0.35737255401129397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="H23">
+        <f>AVERAGE(H4:H21)</f>
+        <v>0.22161519576609984</v>
+      </c>
+      <c r="N23">
+        <f>AVERAGE(N4:N21)</f>
+        <v>6.8095740725405886E-3</v>
+      </c>
+      <c r="T23">
+        <f>AVERAGE(T4:T21)</f>
+        <v>0.27313673394910204</v>
+      </c>
+      <c r="W23">
+        <f>AVERAGE(W4:W21)</f>
+        <v>0.1069924322996211</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="H24">
+        <f>_xlfn.STDEV.S(H4:H21)</f>
+        <v>7.95237246794782E-2</v>
+      </c>
+      <c r="N24">
+        <f>_xlfn.STDEV.S(N4:N21)</f>
+        <v>3.4286685641898469E-3</v>
+      </c>
+      <c r="T24">
+        <f>_xlfn.STDEV.S(T4:T21)</f>
+        <v>0.16319783869030877</v>
+      </c>
+      <c r="W24">
+        <f>_xlfn.STDEV.S(W4:W21)</f>
+        <v>6.1856531982814766E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="H26">
+        <f>AVERAGE(H4:H20)</f>
+        <v>0.22864927312761441</v>
+      </c>
+      <c r="W26">
+        <f>AVERAGE(W4:W20)</f>
+        <v>0.11077052141650863</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>626</v>
+      </c>
+      <c r="B29">
+        <v>6453</v>
+      </c>
+      <c r="E29">
+        <v>672</v>
+      </c>
+      <c r="N29" t="s">
+        <v>626</v>
+      </c>
+      <c r="O29">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>627</v>
+      </c>
+      <c r="B30">
+        <v>4727</v>
+      </c>
+      <c r="E30">
+        <v>892</v>
+      </c>
+      <c r="N30" t="s">
+        <v>627</v>
+      </c>
+      <c r="O30">
+        <v>369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>